<commit_message>
added Excel file to track my prograss
</commit_message>
<xml_diff>
--- a/typing_test_progress_track.xlsx
+++ b/typing_test_progress_track.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t xml:space="preserve">TYPING PRACTICE PROGRESS TRACK</t>
+    <t xml:space="preserve">TYPING TEST PROGRESS TRACK</t>
   </si>
   <si>
     <t>DAYS</t>
@@ -33,16 +33,16 @@
     <t>LESSONS</t>
   </si>
   <si>
-    <t xml:space="preserve">TOP SPEED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVERAGE SPEED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOP ACCURACY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVERAGE ACCURACY</t>
+    <t xml:space="preserve">TOP SPEED (wpm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVERAGE SPEED (wpm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP ACCURACY (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVERAGE ACCURACY (%)</t>
   </si>
   <si>
     <t xml:space="preserve">CURRENT LETTER</t>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -73,13 +73,51 @@
     </font>
     <font>
       <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18.000000"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.000000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18.000000"/>
       <color indexed="2"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="26.000000"/>
+      <sz val="11.000000"/>
       <color indexed="2"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -91,12 +129,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -106,18 +177,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="0"/>
-        <bgColor theme="0" tint="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -125,48 +190,52 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="4" fillId="5" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="4" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="5" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
+    <xf fontId="6" fillId="7" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="7" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="8" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="9" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="9" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="21" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Title" xfId="6" builtinId="15"/>
+    <cellStyle name="Heading 1" xfId="7" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -662,161 +731,121 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="2" style="1" width="13.421875"/>
-    <col customWidth="1" min="3" max="3" style="1" width="14.00390625"/>
-    <col customWidth="1" min="4" max="4" style="1" width="12.7109375"/>
-    <col customWidth="1" min="5" max="5" style="1" width="15.57421875"/>
-    <col customWidth="1" min="6" max="6" style="1" width="14.57421875"/>
-    <col customWidth="1" min="7" max="7" style="1" width="15.57421875"/>
-    <col customWidth="1" min="8" max="8" style="1" width="19.421875"/>
-    <col customWidth="1" min="9" max="9" style="1" width="15.7109375"/>
-    <col min="10" max="10" style="1" width="9.140625"/>
-    <col min="11" max="13" style="1" width="9.140625"/>
-    <col customWidth="1" min="14" max="14" style="1" width="10.28125"/>
-    <col min="15" max="15" style="1" width="9.140625"/>
-    <col min="16" max="56" style="1" width="9.140625"/>
-    <col min="57" max="58" style="1" width="9.140625"/>
-    <col min="59" max="16384" style="1" width="9.140625"/>
+    <col customWidth="1" min="2" max="2" width="11.421875"/>
+    <col customWidth="1" min="3" max="3" width="15.421875"/>
+    <col customWidth="1" min="5" max="5" width="24.421875"/>
+    <col customWidth="1" min="6" max="6" width="22.57421875"/>
+    <col customWidth="1" min="7" max="7" width="19.28125"/>
+    <col customWidth="1" min="8" max="8" width="22.28125"/>
+    <col customWidth="1" min="9" max="9" width="20.140625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" ht="41.25" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3" t="s">
+    <row r="2" ht="31.5" customHeight="1">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-    </row>
-    <row r="3" ht="21" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="BE3" s="6"/>
-      <c r="BF3" s="6"/>
-      <c r="BG3" s="6"/>
-      <c r="BH3" s="6"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="1">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>0.019479166666666665</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>41</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="5">
         <v>45.299999999999997</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>35.200000000000003</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="5">
         <v>98.329999999999998</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="5">
         <v>91.900000000000006</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <v>0.016377314814814813</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>35</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="5">
         <v>41.799999999999997</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>35.600000000000001</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="5">
         <v>100</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="5">
         <v>92.370000000000005</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>

</xml_diff>

<commit_message>
28th Aug | Added other tracking
</commit_message>
<xml_diff>
--- a/typing_test_progress_track.xlsx
+++ b/typing_test_progress_track.xlsx
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">TYPING TEST PROGRESS TRACK</t>
   </si>
   <si>
+    <t>KeyStrokes</t>
+  </si>
+  <si>
     <t>DAYS</t>
   </si>
   <si>
@@ -48,12 +51,33 @@
     <t xml:space="preserve">CURRENT LETTER</t>
   </si>
   <si>
+    <t xml:space="preserve">Typing Test (WPM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">25Th Aug</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
+  </si>
+  <si>
     <t xml:space="preserve">26Th Aug</t>
   </si>
   <si>
@@ -61,13 +85,19 @@
   </si>
   <si>
     <t xml:space="preserve">27Th Aug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28Th Aug</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -120,19 +150,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color indexed="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11.000000"/>
       <color indexed="2"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11.000000"/>
-      <color indexed="5"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +225,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="2"/>
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FFC00000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
   </fills>
@@ -213,23 +282,32 @@
     <xf fontId="5" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
     <xf fontId="6" fillId="7" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="7" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="8" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="9" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="9" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="8" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="8" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="9" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="9" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="10" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="10" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="11" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="21" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="21" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,7 +813,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -743,11 +821,14 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="11.421875"/>
     <col customWidth="1" min="3" max="3" width="15.421875"/>
-    <col customWidth="1" min="5" max="5" width="24.421875"/>
+    <col customWidth="1" min="5" max="5" width="21.140625"/>
     <col customWidth="1" min="6" max="6" width="22.57421875"/>
     <col customWidth="1" min="7" max="7" width="19.28125"/>
     <col customWidth="1" min="8" max="8" width="22.28125"/>
     <col customWidth="1" min="9" max="9" width="20.140625"/>
+    <col customWidth="1" min="10" max="10" width="19.140625"/>
+    <col customWidth="1" min="11" max="11" width="12.8515625"/>
+    <col customWidth="1" min="12" max="12" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="2" ht="31.5" customHeight="1">
@@ -758,126 +839,252 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="2" t="s">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="5">
-        <v>1</v>
+      <c r="A5" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6">
-        <v>0.019479166666666665</v>
-      </c>
-      <c r="D5" s="5">
-        <v>41</v>
-      </c>
-      <c r="E5" s="5">
-        <v>45.299999999999997</v>
-      </c>
-      <c r="F5" s="5">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="G5" s="5">
-        <v>98.329999999999998</v>
-      </c>
-      <c r="H5" s="5">
-        <v>91.900000000000006</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="5">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.016377314814814813</v>
-      </c>
-      <c r="D6" s="5">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5">
-        <v>41.799999999999997</v>
-      </c>
-      <c r="F6" s="5">
-        <v>35.600000000000001</v>
-      </c>
-      <c r="G6" s="5">
-        <v>100</v>
-      </c>
-      <c r="H6" s="5">
-        <v>92.370000000000005</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>13</v>
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.019479166666666665</v>
+      </c>
+      <c r="D6" s="2">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45.299999999999997</v>
+      </c>
+      <c r="F6" s="2">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G6" s="2">
+        <v>98.329999999999998</v>
+      </c>
+      <c r="H6" s="2">
+        <v>91.900000000000006</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.016377314814814813</v>
+      </c>
+      <c r="D7" s="2">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2">
+        <v>41.799999999999997</v>
+      </c>
+      <c r="F7" s="2">
+        <v>35.600000000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>100</v>
+      </c>
+      <c r="H7" s="2">
+        <v>92.370000000000005</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10">
         <v>0.016226851851851853</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="2">
         <v>34</v>
       </c>
-      <c r="E7">
+      <c r="E8" s="2">
         <v>42.600000000000001</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="2">
         <v>34.799999999999997</v>
       </c>
-      <c r="G7">
+      <c r="G8" s="2">
         <v>96.579999999999998</v>
       </c>
-      <c r="H7">
+      <c r="H8" s="2">
         <v>90.969999999999999</v>
       </c>
-      <c r="I7" t="s">
-        <v>13</v>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" ht="14.25">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.016469907407407409</v>
+      </c>
+      <c r="D9" s="2">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2">
+        <v>96.769999999999996</v>
+      </c>
+      <c r="H9" s="2">
+        <v>92.629999999999995</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2">
+        <v>33</v>
+      </c>
+      <c r="K9" s="2">
+        <v>89.129999999999995</v>
+      </c>
+      <c r="L9" s="2">
+        <v>164</v>
+      </c>
+      <c r="M9" s="2">
+        <v>10</v>
+      </c>
+      <c r="N9" s="2">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:G2"/>
+  <mergeCells count="2">
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
2nd Sep typing test score update
</commit_message>
<xml_diff>
--- a/typing_test_progress_track.xlsx
+++ b/typing_test_progress_track.xlsx
@@ -877,7 +877,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1277,11 +1277,11 @@
       <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>26</v>
+      <c r="J14" s="2">
+        <v>44.299999999999997</v>
+      </c>
+      <c r="K14" s="2">
+        <v>96.430000000000007</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
8th Sep typing test score update
</commit_message>
<xml_diff>
--- a/typing_test_progress_track.xlsx
+++ b/typing_test_progress_track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">TYPING TEST PROGRESS TRACK</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">F, Z(ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8th Sep</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
     <xf fontId="5" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
     <xf fontId="6" fillId="7" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="7" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,6 +375,11 @@
     <xf fontId="0" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="11" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="12" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="21" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,7 +885,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="I2" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1293,12 +1301,149 @@
         <v>26</v>
       </c>
     </row>
+    <row r="15" ht="14.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.014733796296296297</v>
+      </c>
+      <c r="D20">
+        <v>31</v>
+      </c>
+      <c r="E20">
+        <v>39.600000000000001</v>
+      </c>
+      <c r="F20">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="G20">
+        <v>96.579999999999998</v>
+      </c>
+      <c r="H20">
+        <v>92.939999999999998</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="G11:I13"/>
+    <mergeCell ref="G16:I19"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>